<commit_message>
Auto update excel file
</commit_message>
<xml_diff>
--- a/all_grants.xlsx
+++ b/all_grants.xlsx
@@ -684,7 +684,7 @@
         </is>
       </c>
       <c r="H2" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" s="1" t="inlineStr">
         <is>
@@ -908,7 +908,7 @@
         </is>
       </c>
       <c r="H3" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" s="1" t="inlineStr">
         <is>
@@ -1117,7 +1117,7 @@
         </is>
       </c>
       <c r="H4" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4" s="1" t="inlineStr">
         <is>
@@ -1168,7 +1168,7 @@
         </is>
       </c>
       <c r="H5" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I5" s="1" t="inlineStr">
         <is>
@@ -1432,7 +1432,7 @@
         </is>
       </c>
       <c r="H6" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6" s="1" t="inlineStr">
         <is>
@@ -1661,7 +1661,7 @@
         </is>
       </c>
       <c r="H7" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7" s="1" t="inlineStr">
         <is>
@@ -1867,7 +1867,7 @@
         </is>
       </c>
       <c r="H8" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I8" s="1" t="inlineStr">
         <is>
@@ -2068,7 +2068,7 @@
         </is>
       </c>
       <c r="H9" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I9" s="1" t="inlineStr">
         <is>
@@ -2275,7 +2275,7 @@
         </is>
       </c>
       <c r="H10" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I10" s="1" t="inlineStr">
         <is>
@@ -2481,7 +2481,7 @@
         </is>
       </c>
       <c r="H11" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I11" s="1" t="inlineStr">
         <is>
@@ -2676,7 +2676,7 @@
         </is>
       </c>
       <c r="H12" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I12" s="1" t="inlineStr">
         <is>
@@ -2890,7 +2890,7 @@
         </is>
       </c>
       <c r="H13" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I13" s="1" t="inlineStr">
         <is>
@@ -3095,7 +3095,7 @@
         </is>
       </c>
       <c r="H14" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I14" s="1" t="inlineStr">
         <is>
@@ -3321,7 +3321,7 @@
         </is>
       </c>
       <c r="H15" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I15" s="1" t="inlineStr">
         <is>
@@ -3549,7 +3549,7 @@
         </is>
       </c>
       <c r="H16" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I16" s="1" t="inlineStr">
         <is>
@@ -3825,7 +3825,7 @@
         </is>
       </c>
       <c r="H17" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I17" s="1" t="inlineStr">
         <is>
@@ -4156,7 +4156,7 @@
         </is>
       </c>
       <c r="H18" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I18" s="1" t="inlineStr">
         <is>
@@ -4357,7 +4357,7 @@
         </is>
       </c>
       <c r="H19" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I19" s="1" t="inlineStr">
         <is>
@@ -4712,7 +4712,7 @@
         </is>
       </c>
       <c r="H20" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I20" s="1" t="inlineStr">
         <is>
@@ -4917,7 +4917,7 @@
         </is>
       </c>
       <c r="H21" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I21" s="1" t="inlineStr">
         <is>
@@ -5124,7 +5124,7 @@
         </is>
       </c>
       <c r="H22" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I22" s="1" t="inlineStr">
         <is>
@@ -5425,7 +5425,7 @@
         </is>
       </c>
       <c r="H23" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I23" s="1" t="inlineStr">
         <is>
@@ -5708,7 +5708,7 @@
         </is>
       </c>
       <c r="H24" s="1" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I24" s="1" t="inlineStr">
         <is>
@@ -5956,7 +5956,7 @@
         </is>
       </c>
       <c r="H25" s="1" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I25" s="1" t="inlineStr">
         <is>
@@ -6167,7 +6167,7 @@
         </is>
       </c>
       <c r="H26" s="1" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I26" s="1" t="inlineStr">
         <is>
@@ -6424,7 +6424,7 @@
         </is>
       </c>
       <c r="H27" s="1" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I27" s="1" t="inlineStr">
         <is>
@@ -6474,7 +6474,7 @@
         </is>
       </c>
       <c r="H28" s="1" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I28" s="1" t="inlineStr">
         <is>
@@ -6672,7 +6672,7 @@
         </is>
       </c>
       <c r="H29" s="1" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I29" s="1" t="inlineStr">
         <is>
@@ -6874,7 +6874,7 @@
         </is>
       </c>
       <c r="H30" s="1" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I30" s="1" t="inlineStr">
         <is>
@@ -7075,7 +7075,7 @@
         </is>
       </c>
       <c r="H31" s="1" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I31" s="1" t="inlineStr">
         <is>
@@ -7322,7 +7322,7 @@
         </is>
       </c>
       <c r="H32" s="1" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I32" s="1" t="inlineStr">
         <is>
@@ -7555,7 +7555,7 @@
         </is>
       </c>
       <c r="H33" s="1" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I33" s="1" t="inlineStr">
         <is>
@@ -7779,7 +7779,7 @@
         </is>
       </c>
       <c r="H34" s="1" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I34" s="1" t="inlineStr">
         <is>
@@ -7985,7 +7985,7 @@
         </is>
       </c>
       <c r="H35" s="1" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I35" s="1" t="inlineStr">
         <is>
@@ -8192,7 +8192,7 @@
         </is>
       </c>
       <c r="H36" s="1" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I36" s="1" t="inlineStr">
         <is>
@@ -8400,7 +8400,7 @@
         </is>
       </c>
       <c r="H37" s="1" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I37" s="1" t="inlineStr">
         <is>

</xml_diff>